<commit_message>
histo analysis, respirometry, and water chem data
</commit_message>
<xml_diff>
--- a/amb_v_constantlow_brood_data/Broodstock_survival_20181112-20190221.xlsx
+++ b/amb_v_constantlow_brood_data/Broodstock_survival_20181112-20190221.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/P_generosa/amb_v_constantlow_brood_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B4EE8C-9837-BE4B-BFEA-78C2717DB29E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D7587-D925-C448-B28A-D25CB520379D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33760" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{01F1A396-36CA-C649-98EC-A8EA62AB1979}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{01F1A396-36CA-C649-98EC-A8EA62AB1979}"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks1-4" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Tanks1-4'!$B$25:$D$25</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Tanks1-4'!$B$33:$D$33</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Tanks1-4'!$B$34:$D$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>TANK</t>
   </si>
@@ -124,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3242,6 +3247,687 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Broodstock survival</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10337331097501701"/>
+          <c:y val="9.7689976995155886E-2"/>
+          <c:w val="0.84665706717215894"/>
+          <c:h val="0.77007331625114561"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Constant low pH (6.8)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Tanks1-4'!$B$63:$E$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.7216146378239299</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.4432292756478695</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10.101525445522084</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Tanks1-4'!$B$63:$E$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.7216146378239299</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.4432292756478695</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>10.101525445522084</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Tanks1-4'!$B$51:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tanks1-4'!$B$59:$E$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.10526315789474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.89473684210526</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.857142857142861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB07-B54C-A887-E6890B745A67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ambient</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Tanks1-4'!$B$64:$E$64</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.7216146378239396</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.186080731891202</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.3367175148507307</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Tanks1-4'!$B$64:$E$64</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.7216146378239396</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.186080731891202</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.3367175148507307</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Tanks1-4'!$B$51:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tanks1-4'!$B$60:$E$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.368421052631575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.868421052631575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.095238095238102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CB07-B54C-A887-E6890B745A67}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1115224351"/>
+        <c:axId val="1115226079"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1115224351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>weeks conditioned</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1115226079"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1115226079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="110"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% survival</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1115224351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2701808634088308"/>
+          <c:y val="0.72250921128920631"/>
+          <c:w val="0.25277847147211296"/>
+          <c:h val="0.10445511332360051"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3522,6 +4208,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6690,6 +7416,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7307,6 +8549,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{546B2AFC-F838-1F42-9CA7-629CFF0B2F32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7607,13 +8885,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDED545C-5189-2844-8325-955D2D1482E2}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="64" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
@@ -7621,7 +8899,7 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -7635,7 +8913,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7655,7 +8933,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -7676,7 +8954,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -7695,7 +8973,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -7714,7 +8992,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -7731,15 +9009,15 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -7749,7 +9027,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -7765,7 +9043,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -7780,7 +9058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -7795,7 +9073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -7810,7 +9088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -7825,7 +9103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -7833,7 +9111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -7847,7 +9125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -7862,7 +9140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -7877,7 +9155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -7892,7 +9170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -7907,7 +9185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -7921,7 +9199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -7938,16 +9216,16 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" ref="B27:B29" si="2">C4/B4*100</f>
+        <f>C4/B4*100</f>
         <v>89.473684210526315</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ref="C27:C29" si="3">C12/B12*100</f>
+        <f>C12/B12*100</f>
         <v>52.631578947368418</v>
       </c>
       <c r="D27" s="1">
@@ -7955,16 +9233,16 @@
         <v>35.714285714285715</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="2"/>
+        <f>C5/B5*100</f>
         <v>94.73684210526315</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="3"/>
+        <f>C13/B13*100</f>
         <v>94.73684210526315</v>
       </c>
       <c r="D28" s="1">
@@ -7972,16 +9250,16 @@
         <v>92.857142857142861</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="2"/>
+        <f>C6/B6*100</f>
         <v>100</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="3"/>
+        <f>C14/B14*100</f>
         <v>95</v>
       </c>
       <c r="D29" s="1">
@@ -7989,12 +9267,12 @@
         <v>93.333333333333329</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -8011,7 +9289,7 @@
         <v>42.857142857142861</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -8028,12 +9306,12 @@
         <v>93.095238095238102</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -8050,7 +9328,7 @@
         <v>10.101525445522084</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -8067,7 +9345,7 @@
         <v>0.3367175148507307</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>28</v>
       </c>
@@ -8075,7 +9353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
@@ -8083,7 +9361,7 @@
         <v>0.70250000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
@@ -8091,7 +9369,7 @@
         <v>3.6470000000000002E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
@@ -8099,7 +9377,7 @@
         <v>2.8289999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
@@ -8107,7 +9385,7 @@
         <v>5.7650000000000002E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -8115,12 +9393,175 @@
         <v>4.0889999999999998E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <v>4</v>
+      </c>
+      <c r="D51" s="1">
+        <v>10</v>
+      </c>
+      <c r="E51" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1">
+        <v>100</v>
+      </c>
+      <c r="C52" s="1">
+        <v>94.73684210526315</v>
+      </c>
+      <c r="D52" s="1">
+        <v>63.157894736842103</v>
+      </c>
+      <c r="E52" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1">
+        <v>100</v>
+      </c>
+      <c r="C53" s="1">
+        <v>89.473684210526315</v>
+      </c>
+      <c r="D53" s="1">
+        <v>52.631578947368418</v>
+      </c>
+      <c r="E53" s="1">
+        <v>35.714285714285715</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1">
+        <v>100</v>
+      </c>
+      <c r="C54" s="1">
+        <v>94.73684210526315</v>
+      </c>
+      <c r="D54" s="1">
+        <v>94.73684210526315</v>
+      </c>
+      <c r="E54" s="1">
+        <v>92.857142857142861</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="1">
+        <v>100</v>
+      </c>
+      <c r="C55" s="1">
+        <v>100</v>
+      </c>
+      <c r="D55" s="1">
+        <v>95</v>
+      </c>
+      <c r="E55" s="1">
+        <v>93.333333333333329</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B59" s="1">
+        <v>100</v>
+      </c>
+      <c r="C59" s="1">
+        <v>92.10526315789474</v>
+      </c>
+      <c r="D59" s="1">
+        <v>57.89473684210526</v>
+      </c>
+      <c r="E59" s="1">
+        <v>42.857142857142861</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="1">
+        <v>100</v>
+      </c>
+      <c r="C60" s="1">
+        <v>97.368421052631575</v>
+      </c>
+      <c r="D60" s="1">
+        <v>94.868421052631575</v>
+      </c>
+      <c r="E60" s="1">
+        <v>93.095238095238102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1">
+        <v>3.7216146378239299</v>
+      </c>
+      <c r="D63" s="1">
+        <v>7.4432292756478695</v>
+      </c>
+      <c r="E63" s="1">
+        <v>10.101525445522084</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3.7216146378239396</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.186080731891202</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.3367175148507307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>